<commit_message>
Add 2025 playoffs data
</commit_message>
<xml_diff>
--- a/NBA_Team_Stats.xlsx
+++ b/NBA_Team_Stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/64ff0ee97f11d84e/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3187d92338a0db9b/Documents/Courses/UNC Courses/665 - Applied Stat II/2025_NBA_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D449DA4-205C-4C3F-A5D0-852C69A04A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{9D449DA4-205C-4C3F-A5D0-852C69A04A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2CD3180-D417-467D-B720-6C5D666A6E37}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26DBB8C9-B1DA-4AA4-8988-B32932631F24}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="11460" windowHeight="14410" xr2:uid="{26DBB8C9-B1DA-4AA4-8988-B32932631F24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -864,11 +864,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA3E85C-50A8-4589-A9EB-F807CE07A312}">
   <dimension ref="A1:Z1285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A565" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="30.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">

</xml_diff>